<commit_message>
App file created and dummy data update
</commit_message>
<xml_diff>
--- a/data/DummyData.xlsx
+++ b/data/DummyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chavezmunoz.a/Documents/Classes/CapstoneC2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00241600-1B55-F94B-8A72-A0B22E95E52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A239FD7E-1A6A-F646-9C8A-D49D92BC5703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10240" yWindow="0" windowWidth="15360" windowHeight="16000" xr2:uid="{AC2BEC5C-A92A-6C4B-8DD5-A07689E57402}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{AC2BEC5C-A92A-6C4B-8DD5-A07689E57402}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="93">
   <si>
     <t>Record ID</t>
   </si>
@@ -68,15 +68,9 @@
     <t>Diabetes</t>
   </si>
   <si>
-    <t>Brachial</t>
-  </si>
-  <si>
     <t>Femoral</t>
   </si>
   <si>
-    <t>Radial</t>
-  </si>
-  <si>
     <t>Popliteal</t>
   </si>
   <si>
@@ -221,9 +215,6 @@
     <t>Cilostazol</t>
   </si>
   <si>
-    <t>Date of Event</t>
-  </si>
-  <si>
     <t>Visit Timepoint</t>
   </si>
   <si>
@@ -314,10 +305,16 @@
     <t>DVA</t>
   </si>
   <si>
-    <t>Cut</t>
-  </si>
-  <si>
-    <t>Wire</t>
+    <t>Tibial</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Endo</t>
+  </si>
+  <si>
+    <t>Date of Thrombosis</t>
   </si>
 </sst>
 </file>
@@ -686,11 +683,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4AB2C12-F0A3-BE48-A042-01696B283B3B}">
   <dimension ref="A1:BR11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AM16" sqref="AM16"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="BR4" sqref="BR4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="19" max="19" width="37.6640625" customWidth="1"/>
+    <col min="20" max="20" width="23.5" customWidth="1"/>
+    <col min="44" max="44" width="21.5" customWidth="1"/>
+    <col min="49" max="49" width="20" customWidth="1"/>
+    <col min="67" max="67" width="17.83203125" customWidth="1"/>
+    <col min="68" max="68" width="19" customWidth="1"/>
+    <col min="69" max="69" width="24.1640625" customWidth="1"/>
+    <col min="70" max="70" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -724,184 +733,184 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="U1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AG1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AM1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AX1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BB1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="BE1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BH1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:70" x14ac:dyDescent="0.2">
@@ -921,10 +930,10 @@
         <v>45000</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="H2" s="2">
         <v>28.5</v>
@@ -936,13 +945,13 @@
         <v>0</v>
       </c>
       <c r="K2" s="2">
-        <v>6.2</v>
+        <v>6</v>
       </c>
       <c r="L2" s="2">
         <v>1</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N2" s="2">
         <v>0</v>
@@ -954,7 +963,7 @@
         <v>0</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R2" s="2">
         <v>0</v>
@@ -998,8 +1007,8 @@
       <c r="AE2" s="2">
         <v>0.91</v>
       </c>
-      <c r="AF2" s="2" t="s">
-        <v>92</v>
+      <c r="AF2" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="AG2" s="2">
         <v>1</v>
@@ -1035,22 +1044,22 @@
         <v>1</v>
       </c>
       <c r="AR2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="AS2" s="2">
         <v>0</v>
       </c>
       <c r="AT2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AU2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AV2" s="3">
         <v>44995</v>
       </c>
       <c r="AW2" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="AX2" s="3">
         <v>44994</v>
@@ -1133,10 +1142,10 @@
         <v>45026</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" s="2">
         <v>32.1</v>
@@ -1148,13 +1157,13 @@
         <v>1</v>
       </c>
       <c r="K3" s="2">
-        <v>7.5</v>
+        <v>7</v>
       </c>
       <c r="L3" s="2">
         <v>0</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N3" s="2">
         <v>1</v>
@@ -1166,7 +1175,7 @@
         <v>1</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="R3" s="2">
         <v>1</v>
@@ -1210,8 +1219,8 @@
       <c r="AE3" s="2">
         <v>0.89</v>
       </c>
-      <c r="AF3" s="2" t="s">
-        <v>93</v>
+      <c r="AF3" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="AG3" s="2">
         <v>0</v>
@@ -1247,22 +1256,20 @@
         <v>0.98</v>
       </c>
       <c r="AR3" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AS3" s="2">
         <v>0</v>
       </c>
       <c r="AT3" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AU3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AV3" s="3">
-        <v>45031</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="AV3" s="3"/>
       <c r="AW3" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AX3" s="3">
         <v>45030</v>
@@ -1345,10 +1352,10 @@
         <v>45066</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="H4" s="2">
         <v>25.8</v>
@@ -1360,13 +1367,13 @@
         <v>0</v>
       </c>
       <c r="K4" s="2">
-        <v>5.9</v>
+        <v>6</v>
       </c>
       <c r="L4" s="2">
         <v>1</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N4" s="2">
         <v>0</v>
@@ -1378,7 +1385,7 @@
         <v>0</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="R4" s="2">
         <v>0</v>
@@ -1422,8 +1429,8 @@
       <c r="AE4" s="2">
         <v>0.94</v>
       </c>
-      <c r="AF4" s="2" t="s">
-        <v>92</v>
+      <c r="AF4" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="AG4" s="2">
         <v>1</v>
@@ -1459,22 +1466,20 @@
         <v>1</v>
       </c>
       <c r="AR4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="AS4" s="2">
         <v>1</v>
       </c>
       <c r="AT4" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AU4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AV4" s="3">
-        <v>45066</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="AV4" s="3"/>
       <c r="AW4" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AX4" s="3">
         <v>45065</v>
@@ -1557,10 +1562,10 @@
         <v>45079</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H5" s="2">
         <v>29.3</v>
@@ -1572,13 +1577,13 @@
         <v>1</v>
       </c>
       <c r="K5" s="2">
-        <v>8.3000000000000007</v>
+        <v>8</v>
       </c>
       <c r="L5" s="2">
         <v>1</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N5" s="2">
         <v>0</v>
@@ -1590,7 +1595,7 @@
         <v>0</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R5" s="2">
         <v>1</v>
@@ -1634,8 +1639,8 @@
       <c r="AE5" s="2">
         <v>0.92</v>
       </c>
-      <c r="AF5" s="2" t="s">
-        <v>93</v>
+      <c r="AF5" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="AG5" s="2">
         <v>0</v>
@@ -1671,22 +1676,22 @@
         <v>0.98</v>
       </c>
       <c r="AR5" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="AS5" s="2">
         <v>0</v>
       </c>
       <c r="AT5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AU5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AV5" s="3">
         <v>45102</v>
       </c>
       <c r="AW5" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AX5" s="3">
         <v>45101</v>
@@ -1769,10 +1774,10 @@
         <v>45118</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="H6" s="2">
         <v>27.2</v>
@@ -1784,13 +1789,13 @@
         <v>0</v>
       </c>
       <c r="K6" s="2">
-        <v>6.7</v>
+        <v>5</v>
       </c>
       <c r="L6" s="2">
         <v>0</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N6" s="2">
         <v>1</v>
@@ -1802,7 +1807,7 @@
         <v>1</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="R6" s="2">
         <v>0</v>
@@ -1846,8 +1851,8 @@
       <c r="AE6" s="2">
         <v>0.91</v>
       </c>
-      <c r="AF6" s="2" t="s">
-        <v>92</v>
+      <c r="AF6" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="AG6" s="2">
         <v>1</v>
@@ -1883,22 +1888,20 @@
         <v>0.99</v>
       </c>
       <c r="AR6" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AS6" s="2">
         <v>0</v>
       </c>
       <c r="AT6" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AU6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AV6" s="3">
-        <v>45137</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="AV6" s="3"/>
       <c r="AW6" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="AX6" s="3">
         <v>45136</v>
@@ -1981,10 +1984,10 @@
         <v>45143</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" s="2">
         <v>31.7</v>
@@ -2002,7 +2005,7 @@
         <v>1</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N7" s="2">
         <v>0</v>
@@ -2014,7 +2017,7 @@
         <v>0</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R7" s="2">
         <v>0</v>
@@ -2058,8 +2061,8 @@
       <c r="AE7" s="2">
         <v>0.9</v>
       </c>
-      <c r="AF7" s="2" t="s">
-        <v>93</v>
+      <c r="AF7" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="AG7" s="2">
         <v>0</v>
@@ -2095,22 +2098,22 @@
         <v>0.97</v>
       </c>
       <c r="AR7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="AS7" s="2">
         <v>1</v>
       </c>
       <c r="AT7" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AU7" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AV7" s="3">
         <v>45143</v>
       </c>
       <c r="AW7" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="AX7" s="3">
         <v>45142</v>
@@ -2193,10 +2196,10 @@
         <v>45183</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="H8" s="2">
         <v>26.9</v>
@@ -2208,13 +2211,13 @@
         <v>0</v>
       </c>
       <c r="K8" s="2">
-        <v>6.8</v>
+        <v>6</v>
       </c>
       <c r="L8" s="2">
         <v>0</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N8" s="2">
         <v>1</v>
@@ -2226,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="R8" s="2">
         <v>0</v>
@@ -2270,8 +2273,8 @@
       <c r="AE8" s="2">
         <v>0.94</v>
       </c>
-      <c r="AF8" s="2" t="s">
-        <v>92</v>
+      <c r="AF8" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="AG8" s="2">
         <v>1</v>
@@ -2307,22 +2310,20 @@
         <v>0.97</v>
       </c>
       <c r="AR8" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AS8" s="2">
         <v>0</v>
       </c>
       <c r="AT8" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AU8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AV8" s="3">
-        <v>45179</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="AV8" s="3"/>
       <c r="AW8" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AX8" s="3">
         <v>45178</v>
@@ -2405,10 +2406,10 @@
         <v>45202</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H9" s="2">
         <v>30.5</v>
@@ -2420,13 +2421,13 @@
         <v>0</v>
       </c>
       <c r="K9" s="2">
-        <v>7.9</v>
+        <v>7</v>
       </c>
       <c r="L9" s="2">
         <v>1</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N9" s="2">
         <v>0</v>
@@ -2438,7 +2439,7 @@
         <v>0</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="R9" s="2">
         <v>1</v>
@@ -2482,8 +2483,8 @@
       <c r="AE9" s="2">
         <v>0.91</v>
       </c>
-      <c r="AF9" s="2" t="s">
-        <v>93</v>
+      <c r="AF9" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="AG9" s="2">
         <v>0</v>
@@ -2519,22 +2520,22 @@
         <v>0.99</v>
       </c>
       <c r="AR9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="AS9" s="2">
         <v>1</v>
       </c>
       <c r="AT9" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AU9" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AV9" s="3">
         <v>45214</v>
       </c>
       <c r="AW9" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AX9" s="3">
         <v>45213</v>
@@ -2617,10 +2618,10 @@
         <v>45252</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="H10" s="2">
         <v>28</v>
@@ -2632,13 +2633,13 @@
         <v>1</v>
       </c>
       <c r="K10" s="2">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="L10" s="2">
         <v>1</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N10" s="2">
         <v>1</v>
@@ -2650,7 +2651,7 @@
         <v>1</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R10" s="2">
         <v>0</v>
@@ -2694,8 +2695,8 @@
       <c r="AE10" s="2">
         <v>0.93</v>
       </c>
-      <c r="AF10" s="2" t="s">
-        <v>92</v>
+      <c r="AF10" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="AG10" s="2">
         <v>1</v>
@@ -2731,22 +2732,20 @@
         <v>1</v>
       </c>
       <c r="AR10" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AS10" s="2">
         <v>0</v>
       </c>
       <c r="AT10" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AU10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AV10" s="3">
-        <v>45250</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="AV10" s="3"/>
       <c r="AW10" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AX10" s="3">
         <v>45249</v>
@@ -2829,10 +2828,10 @@
         <v>45277</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H11" s="2">
         <v>32.4</v>
@@ -2844,13 +2843,13 @@
         <v>0</v>
       </c>
       <c r="K11" s="2">
-        <v>7.2</v>
+        <v>8</v>
       </c>
       <c r="L11" s="2">
         <v>0</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N11" s="2">
         <v>0</v>
@@ -2862,7 +2861,7 @@
         <v>0</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="R11" s="2">
         <v>0</v>
@@ -2906,8 +2905,8 @@
       <c r="AE11" s="2">
         <v>0.92</v>
       </c>
-      <c r="AF11" s="2" t="s">
-        <v>93</v>
+      <c r="AF11" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="AG11" s="2">
         <v>0</v>
@@ -2943,22 +2942,20 @@
         <v>0.96</v>
       </c>
       <c r="AR11" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="AS11" s="2">
         <v>1</v>
       </c>
       <c r="AT11" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AU11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AV11" s="3">
-        <v>45285</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="AV11" s="3"/>
       <c r="AW11" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="AX11" s="3">
         <v>45284</v>

</xml_diff>

<commit_message>
dummy data updated: add none in thr event column
</commit_message>
<xml_diff>
--- a/data/DummyData.xlsx
+++ b/data/DummyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chavezmunoz.a/Documents/Classes/CapstoneC2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77B3327-EA63-294C-8316-9D624DEE9FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DA0238-E51C-7B41-9C71-6DBC8BDEB949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13780" xr2:uid="{AC2BEC5C-A92A-6C4B-8DD5-A07689E57402}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="93">
   <si>
     <t>Record ID</t>
   </si>
@@ -362,11 +362,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4AB2C12-F0A3-BE48-A042-01696B283B3B}">
   <dimension ref="A1:BR11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AU6" sqref="AU6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1267,7 +1268,9 @@
       <c r="AU3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AV3" s="3"/>
+      <c r="AV3" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="AW3" s="2" t="s">
         <v>68</v>
       </c>
@@ -1477,7 +1480,9 @@
       <c r="AU4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AV4" s="3"/>
+      <c r="AV4" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="AW4" s="2" t="s">
         <v>69</v>
       </c>
@@ -1899,7 +1904,9 @@
       <c r="AU6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AV6" s="3"/>
+      <c r="AV6" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="AW6" s="2" t="s">
         <v>71</v>
       </c>
@@ -2321,7 +2328,9 @@
       <c r="AU8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AV8" s="3"/>
+      <c r="AV8" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="AW8" s="2" t="s">
         <v>68</v>
       </c>
@@ -2743,7 +2752,9 @@
       <c r="AU10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AV10" s="3"/>
+      <c r="AV10" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="AW10" s="2" t="s">
         <v>70</v>
       </c>
@@ -2953,7 +2964,9 @@
       <c r="AU11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AV11" s="3"/>
+      <c r="AV11" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="AW11" s="2" t="s">
         <v>71</v>
       </c>

</xml_diff>